<commit_message>
implementing webApi config to load kotlin script functions in memory
</commit_message>
<xml_diff>
--- a/doc/rest-api.xlsx
+++ b/doc/rest-api.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="14920" windowHeight="6910"/>
+    <workbookView activeTab="0" windowWidth="15960" windowHeight="5440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -202,8 +202,10 @@
           <t>send as html, json or text/plain</t>
         </is>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>concat original and posted strings</t>
+        </is>
       </c>
       <c r="D3" s="4" t="s">
         <v>0</v>
@@ -266,7 +268,7 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>execute if there is query string else send html info: parameters and return types</t>
+          <t>return function description</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">

</xml_diff>

<commit_message>
changes to rest api document
</commit_message>
<xml_diff>
--- a/doc/rest-api.xlsx
+++ b/doc/rest-api.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="15960" windowHeight="5440"/>
+    <workbookView activeTab="0" windowWidth="18660" windowHeight="8080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3" count="3">
   <si>
     <t>save data if writable else 403</t>
   </si>
   <si>
     <t>remove resource if allowed else 403</t>
-  </si>
-  <si>
-    <t>400 bad request</t>
   </si>
   <si>
     <t>404 not found</t>
@@ -128,7 +125,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -250,7 +247,7 @@
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>merge if data is entity</t>
+          <t>merge if data is entity or property</t>
         </is>
       </c>
       <c r="D5" s="4" t="s">
@@ -294,8 +291,10 @@
           <t>send toString(value)</t>
         </is>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>2</v>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>400 bad request</t>
+        </is>
       </c>
       <c r="D7" s="4" t="s">
         <v>0</v>
@@ -311,10 +310,10 @@
         </is>
       </c>
       <c r="B8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
@@ -322,7 +321,7 @@
         </is>
       </c>
       <c r="E8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>